<commit_message>
Date filtering, seperated scraping and analysis, company match not found fixed
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atulya\Documents\GitHub\news-sentiment-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46E5ED3-3F11-4114-B9D3-3E8C614C945F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82ECDFB4-2580-4062-9544-8FD8E106FF62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12585" yWindow="2100" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>COMPANYNAME</t>
   </si>
@@ -282,13 +282,43 @@
     <t>https://economictimes.indiatimes.com/markets/stocks/stock-quotes?ticker=</t>
   </si>
   <si>
-    <t>if the company name is not in output - verify company name from here</t>
-  </si>
-  <si>
-    <t>ex. use 'bharti airtel' instead of just 'airtel' for 'Bharti Airtel Ltd.'</t>
-  </si>
-  <si>
     <t>bharat petroleum corp</t>
+  </si>
+  <si>
+    <t>atulya123</t>
+  </si>
+  <si>
+    <t>THRESHOLD</t>
+  </si>
+  <si>
+    <t>icici bank</t>
+  </si>
+  <si>
+    <t>Ideal threshold value between 0.70 to 0.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify company name from - </t>
+  </si>
+  <si>
+    <t>if extra companies are coming in output:</t>
+  </si>
+  <si>
+    <t>modify threshold value or try entering exact name from above URL</t>
+  </si>
+  <si>
+    <t>if the company name is showing NA values in output:</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if output.csv has all keyword counts as 0 </t>
+  </si>
+  <si>
+    <t>check data.csv to verify whether any articles are there in that date range</t>
+  </si>
+  <si>
+    <t>quantiphi</t>
   </si>
 </sst>
 </file>
@@ -358,13 +388,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -651,23 +683,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="71.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" customWidth="1"/>
+    <col min="6" max="6" width="97.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -680,44 +713,54 @@
       <c r="D1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="6">
+        <v>42736</v>
+      </c>
+      <c r="D2" s="6">
+        <v>43647</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>81</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>76</v>
       </c>
@@ -725,167 +768,191 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="F21" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>31</v>
       </c>
@@ -1070,9 +1137,14 @@
         <v>67</v>
       </c>
     </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E13" r:id="rId1" xr:uid="{CA4A3895-C140-4819-8D53-092E3A20D464}"/>
+    <hyperlink ref="F14" r:id="rId1" xr:uid="{622D8AA7-FE82-4DDC-8878-3964154ADB88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
NLTK keyword matching, log creation
similar keywords now counted
log contains urls of articles containing similar keywords
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atulya\Documents\GitHub\news-sentiment-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82ECDFB4-2580-4062-9544-8FD8E106FF62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438377CD-E24E-4B15-BE52-99CEE722A735}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="2100" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>COMPANYNAME</t>
   </si>
@@ -309,16 +309,13 @@
     <t>if the company name is showing NA values in output:</t>
   </si>
   <si>
-    <t>the</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if output.csv has all keyword counts as 0 </t>
-  </si>
-  <si>
     <t>check data.csv to verify whether any articles are there in that date range</t>
   </si>
   <si>
     <t>quantiphi</t>
+  </si>
+  <si>
+    <t>if output.csv has all keyword counts as 0</t>
   </si>
 </sst>
 </file>
@@ -683,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +722,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>94</v>
+        <v>2</v>
       </c>
       <c r="C2" s="6">
         <v>42736</v>
@@ -822,7 +819,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
@@ -891,7 +888,7 @@
         <v>68</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -899,7 +896,7 @@
         <v>20</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1135,11 +1132,6 @@
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moneycontrol scraping done similar to economictimes
Fix Bugs : Stocknames don't appear in some rows
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,24 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atulya\Documents\GitHub\news-sentiment-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438377CD-E24E-4B15-BE52-99CEE722A735}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FE392B-2CDD-4388-A4DC-6C53520EAAA0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t>COMPANYNAME</t>
   </si>
@@ -249,73 +254,58 @@
     <t>WARNING</t>
   </si>
   <si>
-    <t>crisil</t>
-  </si>
-  <si>
-    <t>bharti airtel</t>
+    <t>data.csv</t>
+  </si>
+  <si>
+    <t>output.csv</t>
+  </si>
+  <si>
+    <t>This file can remain open</t>
+  </si>
+  <si>
+    <t>Please close all output files:</t>
+  </si>
+  <si>
+    <t>https://economictimes.indiatimes.com/markets/stocks/stock-quotes?ticker=</t>
+  </si>
+  <si>
+    <t>THRESHOLD</t>
+  </si>
+  <si>
+    <t>Ideal threshold value between 0.70 to 0.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify company name from - </t>
+  </si>
+  <si>
+    <t>if extra companies are coming in output:</t>
+  </si>
+  <si>
+    <t>modify threshold value or try entering exact name from above URL</t>
+  </si>
+  <si>
+    <t>if the company name is showing NA values in output:</t>
+  </si>
+  <si>
+    <t>check data.csv to verify whether any articles are there in that date range</t>
+  </si>
+  <si>
+    <t>if output.csv has all keyword counts as 0</t>
+  </si>
+  <si>
+    <t>WEBSITE</t>
+  </si>
+  <si>
+    <t>economictimes</t>
+  </si>
+  <si>
+    <t>moneycontrol</t>
+  </si>
+  <si>
+    <t>tata steel bsl</t>
   </si>
   <si>
     <t>bank of baroda</t>
-  </si>
-  <si>
-    <t>data.csv</t>
-  </si>
-  <si>
-    <t>output.csv</t>
-  </si>
-  <si>
-    <t>This file can remain open</t>
-  </si>
-  <si>
-    <t>Please close all output files:</t>
-  </si>
-  <si>
-    <t>indiabulls ventures</t>
-  </si>
-  <si>
-    <t>wipro</t>
-  </si>
-  <si>
-    <t>mphasis</t>
-  </si>
-  <si>
-    <t>https://economictimes.indiatimes.com/markets/stocks/stock-quotes?ticker=</t>
-  </si>
-  <si>
-    <t>bharat petroleum corp</t>
-  </si>
-  <si>
-    <t>atulya123</t>
-  </si>
-  <si>
-    <t>THRESHOLD</t>
-  </si>
-  <si>
-    <t>icici bank</t>
-  </si>
-  <si>
-    <t>Ideal threshold value between 0.70 to 0.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verify company name from - </t>
-  </si>
-  <si>
-    <t>if extra companies are coming in output:</t>
-  </si>
-  <si>
-    <t>modify threshold value or try entering exact name from above URL</t>
-  </si>
-  <si>
-    <t>if the company name is showing NA values in output:</t>
-  </si>
-  <si>
-    <t>check data.csv to verify whether any articles are there in that date range</t>
-  </si>
-  <si>
-    <t>quantiphi</t>
-  </si>
-  <si>
-    <t>if output.csv has all keyword counts as 0</t>
   </si>
 </sst>
 </file>
@@ -346,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +361,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -385,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -394,6 +390,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -680,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,11 +691,12 @@
     <col min="3" max="3" width="11.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="2" customWidth="1"/>
-    <col min="6" max="6" width="97.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="97.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -711,245 +710,239 @@
         <v>71</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="6">
-        <v>42736</v>
+        <v>43647</v>
       </c>
       <c r="D2" s="6">
-        <v>43647</v>
+        <v>43656</v>
       </c>
       <c r="E2" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="F2" s="1" t="s">
+        <v>0.75</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>74</v>
-      </c>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="G6" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="G7" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="G8" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>88</v>
-      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>95</v>
-      </c>
+      <c r="G10" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>31</v>
       </c>
@@ -1135,8 +1128,13 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{0FACEBD0-3665-4614-B1EA-3DDDCE1B9749}">
+      <formula1>$G$23:$G$24</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F14" r:id="rId1" xr:uid="{622D8AA7-FE82-4DDC-8878-3964154ADB88}"/>
+    <hyperlink ref="G14" r:id="rId1" xr:uid="{622D8AA7-FE82-4DDC-8878-3964154ADB88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
filename changes, content search by title/article
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atulya\Documents\GitHub\news-sentiment-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA397C7-0384-4A2F-A866-7151BC8F7248}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D237DB5-C106-4F87-BCD1-F53473FDA55F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
   <si>
     <t>COMPANYNAME</t>
   </si>
@@ -309,6 +309,24 @@
   </si>
   <si>
     <t>bhushan steel</t>
+  </si>
+  <si>
+    <t>Article Title</t>
+  </si>
+  <si>
+    <t>Article Content</t>
+  </si>
+  <si>
+    <t>SEARCH OPTION</t>
+  </si>
+  <si>
+    <t>In general this has more contextual meaning accuracy</t>
+  </si>
+  <si>
+    <t>this has benefit of complete scraping</t>
+  </si>
+  <si>
+    <t>WARNING2</t>
   </si>
 </sst>
 </file>
@@ -384,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -395,6 +413,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -681,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,11 +714,13 @@
     <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="97.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="97.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -718,11 +739,17 @@
       <c r="F1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>90</v>
       </c>
@@ -741,11 +768,14 @@
       <c r="F2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>91</v>
       </c>
@@ -755,203 +785,216 @@
       <c r="F3" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3"/>
+      <c r="H3" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="H24" s="9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>31</v>
       </c>
@@ -1137,13 +1180,16 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{0FACEBD0-3665-4614-B1EA-3DDDCE1B9749}">
-      <formula1>$G$23:$G$24</formula1>
+      <formula1>$H$23:$H$24</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{083E63F0-A785-4987-9C26-CD3AEB50D200}">
+      <formula1>$H$26:$H$27</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G14" r:id="rId1" xr:uid="{622D8AA7-FE82-4DDC-8878-3964154ADB88}"/>
+    <hyperlink ref="H14" r:id="rId1" xr:uid="{622D8AA7-FE82-4DDC-8878-3964154ADB88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Bug Fixes and Minor Updates
Fixed proxy=0 and proxy=n condition
Logs printing cleaned
Added error messages when no data is fetched
Fetching previous day and current day stock price seperately
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atulya\Documents\GitHub\news-sentiment-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1948897D-DA3E-415C-A7EE-C121DBBB592B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1762032D-CE63-48F3-A6D7-6A638D82FA65}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
+    <sheet name="temp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="115">
   <si>
     <t>COMPANYNAME</t>
   </si>
@@ -372,6 +373,9 @@
   </si>
   <si>
     <t>ROTATING_PROXIES</t>
+  </si>
+  <si>
+    <t>yes bank</t>
   </si>
 </sst>
 </file>
@@ -760,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +826,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B2" s="4">
         <v>0.8</v>
@@ -837,7 +841,7 @@
         <v>88</v>
       </c>
       <c r="F2" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>2</v>
@@ -856,9 +860,6 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="E3" s="4" t="s">
         <v>89</v>
       </c>
@@ -874,27 +875,18 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="H4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
@@ -903,9 +895,6 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
@@ -914,9 +903,6 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="H8" s="4" t="s">
         <v>8</v>
       </c>
@@ -925,18 +911,12 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="H10" s="4" t="s">
         <v>10</v>
       </c>
@@ -945,18 +925,12 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="H11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="H12" s="4" t="s">
         <v>12</v>
       </c>
@@ -965,9 +939,6 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="H13" s="4" t="s">
         <v>13</v>
       </c>
@@ -976,9 +947,6 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="H14" s="4" t="s">
         <v>14</v>
       </c>
@@ -987,18 +955,12 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>111</v>
-      </c>
       <c r="H15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="H16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1313,4 +1275,100 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2023D26C-8C9A-429C-8A19-EB7B87572914}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A1:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
absolute scoring implemented, sorted scraped data
created score.py
scrape output.csv now sorted first by company name then by descending date
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atulya\Documents\GitHub\news-sentiment-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6225491-9D76-4D34-B069-C542C300F4C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24A9042-32BE-4677-942F-005CF1B0975A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -366,9 +366,6 @@
     <t>ROTATING_PROXIES</t>
   </si>
   <si>
-    <t>POSTITIVE_KEYWORDS</t>
-  </si>
-  <si>
     <t>NEGATIVE_KEYWORDS</t>
   </si>
   <si>
@@ -378,9 +375,6 @@
     <t>volatile</t>
   </si>
   <si>
-    <t>Tata Consultancy services</t>
-  </si>
-  <si>
     <t>tcs</t>
   </si>
   <si>
@@ -409,6 +403,12 @@
   </si>
   <si>
     <t>high performance</t>
+  </si>
+  <si>
+    <t>POSITIVE_KEYWORDS</t>
+  </si>
+  <si>
+    <t>tata consultancy services</t>
   </si>
 </sst>
 </file>
@@ -797,13 +797,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -840,10 +840,10 @@
         <v>110</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>92</v>
@@ -863,7 +863,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="B2" s="4">
         <v>0.8</v>
@@ -886,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>91</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>86</v>
@@ -923,6 +923,9 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
@@ -932,6 +935,9 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>4</v>
       </c>
@@ -941,6 +947,9 @@
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="H6" s="4" t="s">
         <v>5</v>
       </c>
@@ -952,6 +961,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="H7" s="4" t="s">
         <v>6</v>
       </c>
@@ -963,8 +975,11 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="H8" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>12</v>
@@ -974,8 +989,11 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="H9" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>13</v>
@@ -983,8 +1001,11 @@
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="H10" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>14</v>
@@ -994,8 +1015,11 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="H11" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>15</v>
@@ -1003,8 +1027,11 @@
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="H12" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>16</v>
@@ -1014,8 +1041,11 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="H13" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>65</v>
@@ -1025,8 +1055,11 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="H14" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>17</v>
@@ -1036,8 +1069,11 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="H15" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>18</v>
@@ -1045,8 +1081,11 @@
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="H16" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>19</v>
@@ -1055,7 +1094,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="I17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1063,7 +1105,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="I18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1071,13 +1116,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I19" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I20" s="4" t="s">
         <v>23</v>
       </c>
@@ -1085,7 +1130,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I21" s="4" t="s">
         <v>24</v>
       </c>
@@ -1093,13 +1138,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="M22" s="7"/>
     </row>
-    <row r="23" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I23" s="4" t="s">
         <v>26</v>
       </c>
@@ -1107,7 +1152,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I24" s="4" t="s">
         <v>27</v>
       </c>
@@ -1115,12 +1160,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I25" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I26" s="4" t="s">
         <v>29</v>
       </c>
@@ -1131,7 +1176,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I27" s="4" t="s">
         <v>30</v>
       </c>
@@ -1142,27 +1187,27 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I28" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I29" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I30" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I31" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I32" s="4" t="s">
         <v>35</v>
       </c>
@@ -1314,7 +1359,7 @@
     </row>
     <row r="62" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I62" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1381,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2023D26C-8C9A-429C-8A19-EB7B87572914}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A1:A16"/>
@@ -1346,86 +1391,7 @@
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>